<commit_message>
Add run batch file
</commit_message>
<xml_diff>
--- a/USB_Stress_test_kivy_app/Export_data IO-04-001018.xlsx
+++ b/USB_Stress_test_kivy_app/Export_data IO-04-001018.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="97">
   <si>
     <t>Duration</t>
   </si>
@@ -199,31 +199,31 @@
     <t>1470</t>
   </si>
   <si>
-    <t>1500</t>
-  </si>
-  <si>
-    <t>1530</t>
-  </si>
-  <si>
-    <t>1560</t>
-  </si>
-  <si>
-    <t>1590</t>
-  </si>
-  <si>
-    <t>1620</t>
-  </si>
-  <si>
-    <t>1650</t>
-  </si>
-  <si>
-    <t>1680</t>
-  </si>
-  <si>
-    <t>1710</t>
-  </si>
-  <si>
-    <t>1740</t>
+    <t>1499</t>
+  </si>
+  <si>
+    <t>1529</t>
+  </si>
+  <si>
+    <t>1559</t>
+  </si>
+  <si>
+    <t>1589</t>
+  </si>
+  <si>
+    <t>1619</t>
+  </si>
+  <si>
+    <t>1649</t>
+  </si>
+  <si>
+    <t>1679</t>
+  </si>
+  <si>
+    <t>1709</t>
+  </si>
+  <si>
+    <t>1739</t>
   </si>
   <si>
     <t>1770</t>
@@ -235,82 +235,76 @@
     <t>0</t>
   </si>
   <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
     <t>295.41</t>
   </si>
   <si>
+    <t>295.38</t>
+  </si>
+  <si>
+    <t>295.40</t>
+  </si>
+  <si>
+    <t>295.43</t>
+  </si>
+  <si>
+    <t>295.33</t>
+  </si>
+  <si>
+    <t>295.50</t>
+  </si>
+  <si>
+    <t>295.59</t>
+  </si>
+  <si>
     <t>295.39</t>
   </si>
   <si>
-    <t>295.26</t>
-  </si>
-  <si>
-    <t>295.57</t>
+    <t>295.44</t>
   </si>
   <si>
     <t>295.42</t>
   </si>
   <si>
-    <t>295.43</t>
-  </si>
-  <si>
-    <t>295.38</t>
+    <t>295.37</t>
+  </si>
+  <si>
+    <t>295.34</t>
+  </si>
+  <si>
+    <t>295.48</t>
+  </si>
+  <si>
+    <t>295.49</t>
+  </si>
+  <si>
+    <t>295.30</t>
+  </si>
+  <si>
+    <t>295.63</t>
+  </si>
+  <si>
+    <t>295.45</t>
+  </si>
+  <si>
+    <t>295.51</t>
+  </si>
+  <si>
+    <t>295.36</t>
+  </si>
+  <si>
+    <t>295.47</t>
+  </si>
+  <si>
+    <t>295.56</t>
   </si>
   <si>
     <t>295.31</t>
-  </si>
-  <si>
-    <t>295.58</t>
-  </si>
-  <si>
-    <t>295.56</t>
-  </si>
-  <si>
-    <t>295.36</t>
-  </si>
-  <si>
-    <t>295.35</t>
-  </si>
-  <si>
-    <t>295.40</t>
-  </si>
-  <si>
-    <t>295.34</t>
-  </si>
-  <si>
-    <t>295.49</t>
-  </si>
-  <si>
-    <t>295.33</t>
-  </si>
-  <si>
-    <t>295.44</t>
-  </si>
-  <si>
-    <t>295.52</t>
-  </si>
-  <si>
-    <t>295.48</t>
-  </si>
-  <si>
-    <t>295.54</t>
-  </si>
-  <si>
-    <t>295.37</t>
-  </si>
-  <si>
-    <t>295.51</t>
-  </si>
-  <si>
-    <t>295.47</t>
-  </si>
-  <si>
-    <t>295.30</t>
-  </si>
-  <si>
-    <t>295.50</t>
-  </si>
-  <si>
-    <t>295.53</t>
   </si>
 </sst>
 </file>
@@ -738,7 +732,7 @@
         <v>30</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J2" t="s">
         <v>72</v>
@@ -776,10 +770,10 @@
         <v>72</v>
       </c>
       <c r="H3">
-        <v>29.97</v>
+        <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J3" t="s">
         <v>72</v>
@@ -817,10 +811,10 @@
         <v>72</v>
       </c>
       <c r="H4">
-        <v>29.98</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="J4" t="s">
         <v>72</v>
@@ -858,10 +852,10 @@
         <v>72</v>
       </c>
       <c r="H5">
-        <v>29.98</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="J5" t="s">
         <v>72</v>
@@ -899,10 +893,10 @@
         <v>72</v>
       </c>
       <c r="H6">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J6" t="s">
         <v>72</v>
@@ -940,7 +934,7 @@
         <v>72</v>
       </c>
       <c r="H7">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I7" t="s">
         <v>78</v>
@@ -981,7 +975,7 @@
         <v>72</v>
       </c>
       <c r="H8">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I8" t="s">
         <v>79</v>
@@ -1022,10 +1016,10 @@
         <v>72</v>
       </c>
       <c r="H9">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J9" t="s">
         <v>72</v>
@@ -1063,10 +1057,10 @@
         <v>72</v>
       </c>
       <c r="H10">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I10" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="J10" t="s">
         <v>72</v>
@@ -1104,7 +1098,7 @@
         <v>72</v>
       </c>
       <c r="H11">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I11" t="s">
         <v>81</v>
@@ -1145,7 +1139,7 @@
         <v>72</v>
       </c>
       <c r="H12">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I12" t="s">
         <v>82</v>
@@ -1186,10 +1180,10 @@
         <v>72</v>
       </c>
       <c r="H13">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J13" t="s">
         <v>72</v>
@@ -1227,10 +1221,10 @@
         <v>72</v>
       </c>
       <c r="H14">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I14" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="J14" t="s">
         <v>72</v>
@@ -1268,10 +1262,10 @@
         <v>72</v>
       </c>
       <c r="H15">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I15" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="J15" t="s">
         <v>72</v>
@@ -1309,10 +1303,10 @@
         <v>72</v>
       </c>
       <c r="H16">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J16" t="s">
         <v>72</v>
@@ -1350,7 +1344,7 @@
         <v>72</v>
       </c>
       <c r="H17">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I17" t="s">
         <v>84</v>
@@ -1391,10 +1385,10 @@
         <v>72</v>
       </c>
       <c r="H18">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I18" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="J18" t="s">
         <v>72</v>
@@ -1432,10 +1426,10 @@
         <v>72</v>
       </c>
       <c r="H19">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I19" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="J19" t="s">
         <v>72</v>
@@ -1473,7 +1467,7 @@
         <v>72</v>
       </c>
       <c r="H20">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I20" t="s">
         <v>85</v>
@@ -1514,10 +1508,10 @@
         <v>72</v>
       </c>
       <c r="H21">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I21" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="J21" t="s">
         <v>72</v>
@@ -1555,7 +1549,7 @@
         <v>72</v>
       </c>
       <c r="H22">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I22" t="s">
         <v>78</v>
@@ -1596,7 +1590,7 @@
         <v>72</v>
       </c>
       <c r="H23">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I23" t="s">
         <v>86</v>
@@ -1637,7 +1631,7 @@
         <v>72</v>
       </c>
       <c r="H24">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I24" t="s">
         <v>87</v>
@@ -1678,7 +1672,7 @@
         <v>72</v>
       </c>
       <c r="H25">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I25" t="s">
         <v>88</v>
@@ -1719,10 +1713,10 @@
         <v>72</v>
       </c>
       <c r="H26">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I26" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="J26" t="s">
         <v>72</v>
@@ -1760,10 +1754,10 @@
         <v>72</v>
       </c>
       <c r="H27">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I27" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="J27" t="s">
         <v>72</v>
@@ -1801,10 +1795,10 @@
         <v>72</v>
       </c>
       <c r="H28">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I28" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="J28" t="s">
         <v>72</v>
@@ -1824,7 +1818,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>28.01</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
         <v>39</v>
@@ -1842,10 +1836,10 @@
         <v>72</v>
       </c>
       <c r="H29">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I29" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="J29" t="s">
         <v>72</v>
@@ -1865,7 +1859,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>29.01</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
         <v>40</v>
@@ -1883,7 +1877,7 @@
         <v>72</v>
       </c>
       <c r="H30">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I30" t="s">
         <v>89</v>
@@ -1906,7 +1900,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>30.01</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
         <v>41</v>
@@ -1924,10 +1918,10 @@
         <v>72</v>
       </c>
       <c r="H31">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J31" t="s">
         <v>72</v>
@@ -1947,7 +1941,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>31.01</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s">
         <v>42</v>
@@ -1965,10 +1959,10 @@
         <v>72</v>
       </c>
       <c r="H32">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I32" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="J32" t="s">
         <v>72</v>
@@ -1988,7 +1982,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>32.01</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s">
         <v>43</v>
@@ -2009,7 +2003,7 @@
         <v>30</v>
       </c>
       <c r="I33" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="J33" t="s">
         <v>72</v>
@@ -2029,7 +2023,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>33.01</v>
+        <v>33</v>
       </c>
       <c r="C34" t="s">
         <v>44</v>
@@ -2050,7 +2044,7 @@
         <v>30</v>
       </c>
       <c r="I34" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J34" t="s">
         <v>72</v>
@@ -2070,7 +2064,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>34.01</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s">
         <v>45</v>
@@ -2091,7 +2085,7 @@
         <v>30</v>
       </c>
       <c r="I35" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J35" t="s">
         <v>72</v>
@@ -2111,7 +2105,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>35.01</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s">
         <v>46</v>
@@ -2152,7 +2146,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>36.01</v>
+        <v>36</v>
       </c>
       <c r="C37" t="s">
         <v>47</v>
@@ -2173,7 +2167,7 @@
         <v>30</v>
       </c>
       <c r="I37" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="J37" t="s">
         <v>72</v>
@@ -2193,7 +2187,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>37.01</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s">
         <v>48</v>
@@ -2214,7 +2208,7 @@
         <v>30</v>
       </c>
       <c r="I38" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J38" t="s">
         <v>72</v>
@@ -2234,7 +2228,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>38.01</v>
+        <v>38</v>
       </c>
       <c r="C39" t="s">
         <v>49</v>
@@ -2275,7 +2269,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>39.01</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
         <v>50</v>
@@ -2296,7 +2290,7 @@
         <v>30</v>
       </c>
       <c r="I40" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="J40" t="s">
         <v>72</v>
@@ -2316,7 +2310,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>40.01</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s">
         <v>51</v>
@@ -2357,7 +2351,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>41.01</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s">
         <v>52</v>
@@ -2378,7 +2372,7 @@
         <v>30</v>
       </c>
       <c r="I42" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="J42" t="s">
         <v>72</v>
@@ -2398,7 +2392,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>42.01</v>
+        <v>42</v>
       </c>
       <c r="C43" t="s">
         <v>53</v>
@@ -2419,7 +2413,7 @@
         <v>30</v>
       </c>
       <c r="I43" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="J43" t="s">
         <v>72</v>
@@ -2439,7 +2433,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>43.01</v>
+        <v>43</v>
       </c>
       <c r="C44" t="s">
         <v>54</v>
@@ -2460,7 +2454,7 @@
         <v>30</v>
       </c>
       <c r="I44" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="J44" t="s">
         <v>72</v>
@@ -2480,7 +2474,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>44.01</v>
+        <v>44</v>
       </c>
       <c r="C45" t="s">
         <v>55</v>
@@ -2501,7 +2495,7 @@
         <v>30</v>
       </c>
       <c r="I45" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="J45" t="s">
         <v>72</v>
@@ -2521,7 +2515,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>45.01</v>
+        <v>45</v>
       </c>
       <c r="C46" t="s">
         <v>56</v>
@@ -2542,7 +2536,7 @@
         <v>30</v>
       </c>
       <c r="I46" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="J46" t="s">
         <v>72</v>
@@ -2562,7 +2556,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>46.01</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
         <v>57</v>
@@ -2583,7 +2577,7 @@
         <v>30</v>
       </c>
       <c r="I47" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J47" t="s">
         <v>72</v>
@@ -2603,7 +2597,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>47.01</v>
+        <v>47</v>
       </c>
       <c r="C48" t="s">
         <v>58</v>
@@ -2624,7 +2618,7 @@
         <v>30</v>
       </c>
       <c r="I48" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="J48" t="s">
         <v>72</v>
@@ -2644,7 +2638,7 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>48.01</v>
+        <v>48</v>
       </c>
       <c r="C49" t="s">
         <v>59</v>
@@ -2665,7 +2659,7 @@
         <v>30</v>
       </c>
       <c r="I49" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="J49" t="s">
         <v>72</v>
@@ -2685,7 +2679,7 @@
         <v>48</v>
       </c>
       <c r="B50">
-        <v>49.01</v>
+        <v>49</v>
       </c>
       <c r="C50" t="s">
         <v>60</v>
@@ -2706,7 +2700,7 @@
         <v>30</v>
       </c>
       <c r="I50" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="J50" t="s">
         <v>72</v>
@@ -2726,7 +2720,7 @@
         <v>49</v>
       </c>
       <c r="B51">
-        <v>50.01</v>
+        <v>50</v>
       </c>
       <c r="C51" t="s">
         <v>61</v>
@@ -2738,16 +2732,16 @@
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>12</v>
+        <v>73</v>
       </c>
       <c r="G51" t="s">
         <v>72</v>
       </c>
       <c r="H51">
-        <v>30</v>
+        <v>29.98</v>
       </c>
       <c r="I51" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="J51" t="s">
         <v>72</v>
@@ -2767,7 +2761,7 @@
         <v>50</v>
       </c>
       <c r="B52">
-        <v>51.01</v>
+        <v>51</v>
       </c>
       <c r="C52" t="s">
         <v>62</v>
@@ -2785,10 +2779,10 @@
         <v>72</v>
       </c>
       <c r="H52">
-        <v>30</v>
+        <v>29.98</v>
       </c>
       <c r="I52" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="J52" t="s">
         <v>72</v>
@@ -2808,7 +2802,7 @@
         <v>51</v>
       </c>
       <c r="B53">
-        <v>52.01</v>
+        <v>52</v>
       </c>
       <c r="C53" t="s">
         <v>63</v>
@@ -2826,10 +2820,10 @@
         <v>72</v>
       </c>
       <c r="H53">
-        <v>30</v>
+        <v>29.98</v>
       </c>
       <c r="I53" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="J53" t="s">
         <v>72</v>
@@ -2849,7 +2843,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>53.01</v>
+        <v>53</v>
       </c>
       <c r="C54" t="s">
         <v>64</v>
@@ -2867,10 +2861,10 @@
         <v>72</v>
       </c>
       <c r="H54">
-        <v>30</v>
+        <v>29.98</v>
       </c>
       <c r="I54" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="J54" t="s">
         <v>72</v>
@@ -2890,7 +2884,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>54.01</v>
+        <v>54</v>
       </c>
       <c r="C55" t="s">
         <v>65</v>
@@ -2908,10 +2902,10 @@
         <v>72</v>
       </c>
       <c r="H55">
-        <v>30</v>
+        <v>29.98</v>
       </c>
       <c r="I55" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="J55" t="s">
         <v>72</v>
@@ -2931,7 +2925,7 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>55.01</v>
+        <v>55</v>
       </c>
       <c r="C56" t="s">
         <v>66</v>
@@ -2949,10 +2943,10 @@
         <v>72</v>
       </c>
       <c r="H56">
-        <v>30</v>
+        <v>29.98</v>
       </c>
       <c r="I56" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J56" t="s">
         <v>72</v>
@@ -2972,7 +2966,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>56.01</v>
+        <v>56</v>
       </c>
       <c r="C57" t="s">
         <v>67</v>
@@ -2990,10 +2984,10 @@
         <v>72</v>
       </c>
       <c r="H57">
-        <v>30</v>
+        <v>29.98</v>
       </c>
       <c r="I57" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J57" t="s">
         <v>72</v>
@@ -3013,7 +3007,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>57.01</v>
+        <v>57</v>
       </c>
       <c r="C58" t="s">
         <v>68</v>
@@ -3031,10 +3025,10 @@
         <v>72</v>
       </c>
       <c r="H58">
-        <v>30</v>
+        <v>29.98</v>
       </c>
       <c r="I58" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J58" t="s">
         <v>72</v>
@@ -3054,7 +3048,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>58.01</v>
+        <v>58</v>
       </c>
       <c r="C59" t="s">
         <v>69</v>
@@ -3072,7 +3066,7 @@
         <v>72</v>
       </c>
       <c r="H59">
-        <v>30</v>
+        <v>29.98</v>
       </c>
       <c r="I59" t="s">
         <v>78</v>
@@ -3107,7 +3101,7 @@
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>12</v>
+        <v>74</v>
       </c>
       <c r="G60" t="s">
         <v>72</v>
@@ -3116,7 +3110,7 @@
         <v>30</v>
       </c>
       <c r="I60" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="J60" t="s">
         <v>72</v>
@@ -3157,7 +3151,7 @@
         <v>30</v>
       </c>
       <c r="I61" t="s">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="J61" t="s">
         <v>72</v>
@@ -3198,7 +3192,7 @@
         <v>30</v>
       </c>
       <c r="I62" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J62" t="s">
         <v>72</v>
@@ -3239,7 +3233,7 @@
         <v>30</v>
       </c>
       <c r="I63" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="J63" t="s">
         <v>72</v>
@@ -3280,7 +3274,7 @@
         <v>30</v>
       </c>
       <c r="I64" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J64" t="s">
         <v>72</v>
@@ -3362,7 +3356,7 @@
         <v>30</v>
       </c>
       <c r="I66" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J66" t="s">
         <v>72</v>
@@ -3403,7 +3397,7 @@
         <v>30</v>
       </c>
       <c r="I67" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="J67" t="s">
         <v>72</v>
@@ -3444,7 +3438,7 @@
         <v>30</v>
       </c>
       <c r="I68" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="J68" t="s">
         <v>72</v>
@@ -3485,7 +3479,7 @@
         <v>30</v>
       </c>
       <c r="I69" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="J69" t="s">
         <v>72</v>
@@ -3526,7 +3520,7 @@
         <v>30</v>
       </c>
       <c r="I70" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="J70" t="s">
         <v>72</v>
@@ -3567,7 +3561,7 @@
         <v>30</v>
       </c>
       <c r="I71" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="J71" t="s">
         <v>72</v>
@@ -3608,7 +3602,7 @@
         <v>30</v>
       </c>
       <c r="I72" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="J72" t="s">
         <v>72</v>
@@ -3690,7 +3684,7 @@
         <v>30</v>
       </c>
       <c r="I74" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J74" t="s">
         <v>72</v>
@@ -3731,7 +3725,7 @@
         <v>30</v>
       </c>
       <c r="I75" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J75" t="s">
         <v>72</v>
@@ -3772,7 +3766,7 @@
         <v>30</v>
       </c>
       <c r="I76" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J76" t="s">
         <v>72</v>
@@ -3813,7 +3807,7 @@
         <v>30</v>
       </c>
       <c r="I77" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="J77" t="s">
         <v>72</v>
@@ -3854,7 +3848,7 @@
         <v>30</v>
       </c>
       <c r="I78" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="J78" t="s">
         <v>72</v>
@@ -3895,7 +3889,7 @@
         <v>30</v>
       </c>
       <c r="I79" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="J79" t="s">
         <v>72</v>
@@ -3936,7 +3930,7 @@
         <v>30</v>
       </c>
       <c r="I80" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="J80" t="s">
         <v>72</v>
@@ -3977,7 +3971,7 @@
         <v>30</v>
       </c>
       <c r="I81" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="J81" t="s">
         <v>72</v>
@@ -4018,7 +4012,7 @@
         <v>30</v>
       </c>
       <c r="I82" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="J82" t="s">
         <v>72</v>
@@ -4059,7 +4053,7 @@
         <v>30</v>
       </c>
       <c r="I83" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="J83" t="s">
         <v>72</v>
@@ -4100,7 +4094,7 @@
         <v>30</v>
       </c>
       <c r="I84" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J84" t="s">
         <v>72</v>
@@ -4141,7 +4135,7 @@
         <v>30</v>
       </c>
       <c r="I85" t="s">
-        <v>77</v>
+        <v>92</v>
       </c>
       <c r="J85" t="s">
         <v>72</v>
@@ -4182,7 +4176,7 @@
         <v>30</v>
       </c>
       <c r="I86" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="J86" t="s">
         <v>72</v>
@@ -4220,10 +4214,10 @@
         <v>72</v>
       </c>
       <c r="H87">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I87" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J87" t="s">
         <v>72</v>
@@ -4261,10 +4255,10 @@
         <v>72</v>
       </c>
       <c r="H88">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I88" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="J88" t="s">
         <v>72</v>
@@ -4302,10 +4296,10 @@
         <v>72</v>
       </c>
       <c r="H89">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I89" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="J89" t="s">
         <v>72</v>
@@ -4325,7 +4319,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>29.01</v>
+        <v>29</v>
       </c>
       <c r="C90" t="s">
         <v>40</v>
@@ -4343,10 +4337,10 @@
         <v>72</v>
       </c>
       <c r="H90">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I90" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="J90" t="s">
         <v>72</v>
@@ -4366,7 +4360,7 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>30.01</v>
+        <v>30</v>
       </c>
       <c r="C91" t="s">
         <v>41</v>
@@ -4384,10 +4378,10 @@
         <v>72</v>
       </c>
       <c r="H91">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I91" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J91" t="s">
         <v>72</v>
@@ -4407,7 +4401,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>31.01</v>
+        <v>31</v>
       </c>
       <c r="C92" t="s">
         <v>42</v>
@@ -4425,10 +4419,10 @@
         <v>72</v>
       </c>
       <c r="H92">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I92" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="J92" t="s">
         <v>72</v>
@@ -4448,7 +4442,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>32.01</v>
+        <v>32</v>
       </c>
       <c r="C93" t="s">
         <v>43</v>
@@ -4469,7 +4463,7 @@
         <v>30</v>
       </c>
       <c r="I93" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="J93" t="s">
         <v>72</v>
@@ -4489,7 +4483,7 @@
         <v>92</v>
       </c>
       <c r="B94">
-        <v>33.01</v>
+        <v>33</v>
       </c>
       <c r="C94" t="s">
         <v>44</v>
@@ -4530,7 +4524,7 @@
         <v>93</v>
       </c>
       <c r="B95">
-        <v>34.01</v>
+        <v>34</v>
       </c>
       <c r="C95" t="s">
         <v>45</v>
@@ -4551,7 +4545,7 @@
         <v>30</v>
       </c>
       <c r="I95" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="J95" t="s">
         <v>72</v>
@@ -4571,7 +4565,7 @@
         <v>94</v>
       </c>
       <c r="B96">
-        <v>35.01</v>
+        <v>35</v>
       </c>
       <c r="C96" t="s">
         <v>46</v>
@@ -4592,7 +4586,7 @@
         <v>30</v>
       </c>
       <c r="I96" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="J96" t="s">
         <v>72</v>
@@ -4612,7 +4606,7 @@
         <v>95</v>
       </c>
       <c r="B97">
-        <v>36.01</v>
+        <v>36</v>
       </c>
       <c r="C97" t="s">
         <v>47</v>
@@ -4633,7 +4627,7 @@
         <v>30</v>
       </c>
       <c r="I97" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="J97" t="s">
         <v>72</v>
@@ -4653,7 +4647,7 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>37.01</v>
+        <v>37</v>
       </c>
       <c r="C98" t="s">
         <v>48</v>
@@ -4674,7 +4668,7 @@
         <v>30</v>
       </c>
       <c r="I98" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="J98" t="s">
         <v>72</v>
@@ -4694,7 +4688,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>38.01</v>
+        <v>38</v>
       </c>
       <c r="C99" t="s">
         <v>49</v>
@@ -4715,7 +4709,7 @@
         <v>30</v>
       </c>
       <c r="I99" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="J99" t="s">
         <v>72</v>
@@ -4735,7 +4729,7 @@
         <v>98</v>
       </c>
       <c r="B100">
-        <v>39.01</v>
+        <v>39</v>
       </c>
       <c r="C100" t="s">
         <v>50</v>
@@ -4753,10 +4747,10 @@
         <v>72</v>
       </c>
       <c r="H100">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I100" t="s">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="J100" t="s">
         <v>72</v>
@@ -4776,7 +4770,7 @@
         <v>99</v>
       </c>
       <c r="B101">
-        <v>40.01</v>
+        <v>40</v>
       </c>
       <c r="C101" t="s">
         <v>51</v>
@@ -4794,10 +4788,10 @@
         <v>72</v>
       </c>
       <c r="H101">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I101" t="s">
-        <v>77</v>
+        <v>95</v>
       </c>
       <c r="J101" t="s">
         <v>72</v>
@@ -4817,7 +4811,7 @@
         <v>100</v>
       </c>
       <c r="B102">
-        <v>41.01</v>
+        <v>41</v>
       </c>
       <c r="C102" t="s">
         <v>52</v>
@@ -4835,10 +4829,10 @@
         <v>72</v>
       </c>
       <c r="H102">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I102" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J102" t="s">
         <v>72</v>
@@ -4858,7 +4852,7 @@
         <v>101</v>
       </c>
       <c r="B103">
-        <v>42.01</v>
+        <v>42</v>
       </c>
       <c r="C103" t="s">
         <v>53</v>
@@ -4876,10 +4870,10 @@
         <v>72</v>
       </c>
       <c r="H103">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I103" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="J103" t="s">
         <v>72</v>
@@ -4899,7 +4893,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>43.01</v>
+        <v>43</v>
       </c>
       <c r="C104" t="s">
         <v>54</v>
@@ -4917,7 +4911,7 @@
         <v>72</v>
       </c>
       <c r="H104">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I104" t="s">
         <v>78</v>
@@ -4940,7 +4934,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>44.01</v>
+        <v>44</v>
       </c>
       <c r="C105" t="s">
         <v>55</v>
@@ -4958,10 +4952,10 @@
         <v>72</v>
       </c>
       <c r="H105">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I105" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J105" t="s">
         <v>72</v>
@@ -4981,7 +4975,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>45.01</v>
+        <v>45</v>
       </c>
       <c r="C106" t="s">
         <v>56</v>
@@ -4999,10 +4993,10 @@
         <v>72</v>
       </c>
       <c r="H106">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I106" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="J106" t="s">
         <v>72</v>
@@ -5022,7 +5016,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>46.01</v>
+        <v>46</v>
       </c>
       <c r="C107" t="s">
         <v>57</v>
@@ -5040,10 +5034,10 @@
         <v>72</v>
       </c>
       <c r="H107">
-        <v>29.99</v>
+        <v>30</v>
       </c>
       <c r="I107" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="J107" t="s">
         <v>72</v>
@@ -5063,7 +5057,7 @@
         <v>106</v>
       </c>
       <c r="B108">
-        <v>47.01</v>
+        <v>47</v>
       </c>
       <c r="C108" t="s">
         <v>58</v>
@@ -5084,7 +5078,7 @@
         <v>30</v>
       </c>
       <c r="I108" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="J108" t="s">
         <v>72</v>
@@ -5104,7 +5098,7 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>48.01</v>
+        <v>48</v>
       </c>
       <c r="C109" t="s">
         <v>59</v>
@@ -5125,7 +5119,7 @@
         <v>30</v>
       </c>
       <c r="I109" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J109" t="s">
         <v>72</v>
@@ -5145,7 +5139,7 @@
         <v>108</v>
       </c>
       <c r="B110">
-        <v>49.01</v>
+        <v>49</v>
       </c>
       <c r="C110" t="s">
         <v>60</v>
@@ -5166,7 +5160,7 @@
         <v>30</v>
       </c>
       <c r="I110" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="J110" t="s">
         <v>72</v>

</xml_diff>